<commit_message>
2022 F1040 Schedule 1
</commit_message>
<xml_diff>
--- a/Federal/f1040s1-2022.xlsx
+++ b/Federal/f1040s1-2022.xlsx
@@ -1101,45 +1101,79 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1465,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:H36"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1477,1168 +1511,1204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="11" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="1" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="12"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="1" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="12"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="1" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="12"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="1" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="1" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J9" s="12"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="1" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="12"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="1" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J11" s="12"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="24">
+      <c r="A12" s="17">
         <v>8</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="20"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="1" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="17"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="20"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="1" t="s">
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="17"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="20"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="1" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="17"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="20"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="1" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="1" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="17"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="20"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="1" t="s">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="20"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="1" t="s">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="17"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="20"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="1" t="s">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="17"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="1" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="17"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="1" t="s">
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="17"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="1" t="s">
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="17"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="1" t="s">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="17"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="1" t="s">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="17"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="1" t="s">
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="3"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="17"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="1" t="s">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="17"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="1" t="s">
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="17"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="H28" s="22"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="20"/>
+    </row>
+    <row r="29" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="1" t="s">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="H29" s="3"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="17"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="H29" s="22"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="20"/>
+    </row>
+    <row r="30" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="1" t="s">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H30" s="3"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="17"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="1" t="s">
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H31" s="3"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="17"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="1" t="s">
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H32" s="3"/>
-      <c r="I32" s="16"/>
-      <c r="J32" s="17"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="20"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="1" t="s">
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="17"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="20"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="1" t="s">
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H34" s="3"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="17"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="20"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="1" t="s">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="J35" s="12">
+      <c r="J35" s="5">
         <f>SUM(H13:H34)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="20" t="s">
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="J36" s="21"/>
+      <c r="J36" s="8">
+        <f>SUM(J5:J35)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="11" t="s">
         <v>2</v>
       </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="23"/>
+      <c r="J38" s="23"/>
     </row>
     <row r="39" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="A39" s="11" t="s">
         <v>2</v>
       </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="10"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="14"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="1" t="s">
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="J41" s="12"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="1" t="s">
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="J42" s="12"/>
+      <c r="J42" s="5"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="1" t="s">
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="J43" s="12"/>
+      <c r="J43" s="5"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="1" t="s">
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J44" s="12"/>
+      <c r="J44" s="5"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="1" t="s">
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J45" s="12"/>
+      <c r="J45" s="5"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="1" t="s">
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="J46" s="12"/>
+      <c r="J46" s="5"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="1" t="s">
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="J47" s="12"/>
+      <c r="J47" s="5"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="1" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="J48" s="12"/>
+      <c r="J48" s="5"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="1" t="s">
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="J49" s="12"/>
+      <c r="J49" s="5"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="1" t="s">
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J50" s="12"/>
+      <c r="J50" s="5"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="1" t="s">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J51" s="12"/>
+      <c r="J51" s="5"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+      <c r="A52" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="1" t="s">
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="J52" s="12"/>
+      <c r="J52" s="5"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
+      <c r="A53" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="1" t="s">
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="J53" s="12"/>
+      <c r="J53" s="5"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="7">
+      <c r="A54" s="24">
         <v>24</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="15"/>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="20"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="1" t="s">
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="H55" s="3"/>
-      <c r="I55" s="16"/>
-      <c r="J55" s="17"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
+      <c r="H55" s="22"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="20"/>
+    </row>
+    <row r="56" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="1" t="s">
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="H56" s="3"/>
-      <c r="I56" s="16"/>
-      <c r="J56" s="17"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
+      <c r="H56" s="22"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="20"/>
+    </row>
+    <row r="57" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="1" t="s">
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="H57" s="3"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="17"/>
+      <c r="H57" s="22"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="20"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="1" t="s">
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="H58" s="3"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="17"/>
+      <c r="H58" s="22"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="20"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="1" t="s">
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H59" s="3"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="17"/>
+      <c r="H59" s="22"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="20"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="A60" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="1" t="s">
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="H60" s="3"/>
-      <c r="I60" s="16"/>
-      <c r="J60" s="17"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="20"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="A61" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="1" t="s">
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="H61" s="3"/>
-      <c r="I61" s="16"/>
-      <c r="J61" s="17"/>
+      <c r="H61" s="22"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="20"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
+      <c r="A62" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="1" t="s">
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="H62" s="3"/>
-      <c r="I62" s="16"/>
-      <c r="J62" s="17"/>
+      <c r="H62" s="22"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="20"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="1" t="s">
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H63" s="3"/>
-      <c r="I63" s="16"/>
-      <c r="J63" s="17"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="20"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="1" t="s">
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="H64" s="3"/>
-      <c r="I64" s="16"/>
-      <c r="J64" s="17"/>
+      <c r="H64" s="22"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="20"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
+      <c r="A65" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="1" t="s">
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="H65" s="3"/>
-      <c r="I65" s="16"/>
-      <c r="J65" s="17"/>
+      <c r="H65" s="22"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="20"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="1" t="s">
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H66" s="3"/>
-      <c r="I66" s="16"/>
-      <c r="J66" s="17"/>
+      <c r="H66" s="22"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="20"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="1" t="s">
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="J67" s="12"/>
-    </row>
-    <row r="68" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="18" t="s">
+      <c r="J67" s="5">
+        <f>SUM(H55:H66)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="B68" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C68" s="19"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="19"/>
-      <c r="F68" s="19"/>
-      <c r="G68" s="19"/>
-      <c r="H68" s="19"/>
-      <c r="I68" s="20" t="s">
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="J68" s="21"/>
+      <c r="J68" s="8">
+        <f>SUM(J41:J67)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -2647,16 +2717,42 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:H67"/>
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B54:H54"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="B59:F59"/>
-    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="A38:J38"/>
     <mergeCell ref="B61:F61"/>
     <mergeCell ref="B62:F62"/>
     <mergeCell ref="B63:F63"/>
@@ -2665,6 +2761,11 @@
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="B56:F56"/>
     <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B54:H54"/>
+    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B60:F60"/>
     <mergeCell ref="B46:H46"/>
     <mergeCell ref="B47:H47"/>
     <mergeCell ref="B48:H48"/>
@@ -2676,42 +2777,11 @@
     <mergeCell ref="B42:H42"/>
     <mergeCell ref="B43:H43"/>
     <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="A38:J38"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B67:H67"/>
+    <mergeCell ref="B68:H68"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>